<commit_message>
setting warna ke ukuran
</commit_message>
<xml_diff>
--- a/public/files/template.xlsx
+++ b/public/files/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deva satrio\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\git\TA\public\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -41,9 +41,6 @@
     <t>stok</t>
   </si>
   <si>
-    <t>warna</t>
-  </si>
-  <si>
     <t>varian</t>
   </si>
   <si>
@@ -54,6 +51,9 @@
   </si>
   <si>
     <t>harga_beli</t>
+  </si>
+  <si>
+    <t>ukuran</t>
   </si>
 </sst>
 </file>
@@ -378,7 +378,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -403,19 +403,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>3</v>
@@ -423,7 +423,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
build up new tastore
</commit_message>
<xml_diff>
--- a/public/files/template.xlsx
+++ b/public/files/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\git\TA\public\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deva satrio\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -41,6 +41,9 @@
     <t>stok</t>
   </si>
   <si>
+    <t>warna</t>
+  </si>
+  <si>
     <t>varian</t>
   </si>
   <si>
@@ -51,9 +54,6 @@
   </si>
   <si>
     <t>harga_beli</t>
-  </si>
-  <si>
-    <t>ukuran</t>
   </si>
 </sst>
 </file>
@@ -378,7 +378,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -403,19 +403,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>3</v>
@@ -423,7 +423,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>